<commit_message>
Add EPJ standard del 1 schemas, Add overview pdf.
</commit_message>
<xml_diff>
--- a/oversikt_2.16.578.1.39.100.10.1047.1.5.xlsx
+++ b/oversikt_2.16.578.1.39.100.10.1047.1.5.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://arkivverket-my.sharepoint.com/personal/areant_arkivverket_no/Documents/Documents/DPS/EPJ/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\areant\work\epj-testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{EFA12068-DFC4-443E-8615-73B1B9CB0D7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{08B8AFDE-D779-45D2-83E5-200C5F6DE9C4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E309FE-4C08-410B-865C-EB6EDD023ADF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{9C01A0FA-149D-445D-84EE-C26FA580F441}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$F$26</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -691,151 +694,151 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1152,10 +1155,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E73E85-BA29-40E5-ADC9-643B2746FE37}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection sqref="A1:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,224 +1181,224 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="46" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="9" t="s">
+      <c r="A4" s="44"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="47"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="8" t="s">
+      <c r="A5" s="44"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="47"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="17" t="s">
+      <c r="A6" s="44"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19" t="s">
+      <c r="D6" s="15"/>
+      <c r="E6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="34" t="s">
+      <c r="A7" s="44"/>
+      <c r="B7" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="46" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="11" t="s">
+      <c r="A8" s="44"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="6"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="47"/>
     </row>
     <row r="9" spans="1:6" ht="240" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="11" t="s">
+      <c r="A9" s="44"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="6"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="47"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="18" t="s">
+      <c r="A10" s="44"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19" t="s">
+      <c r="D10" s="15"/>
+      <c r="E10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="47"/>
     </row>
     <row r="11" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="34" t="s">
+      <c r="A11" s="44"/>
+      <c r="B11" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="3" t="s">
+      <c r="E11" s="11"/>
+      <c r="F11" s="46" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="25" t="s">
+      <c r="A12" s="44"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="47"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="8" t="s">
+      <c r="A13" s="44"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="47"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="17" t="s">
+      <c r="A14" s="44"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19" t="s">
+      <c r="D14" s="15"/>
+      <c r="E14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="47"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="30" t="s">
+      <c r="A15" s="44"/>
+      <c r="B15" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30" t="s">
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="24" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="30" t="s">
+      <c r="A16" s="44"/>
+      <c r="B16" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30" t="s">
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="24" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="24"/>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="45"/>
+      <c r="B17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="32" t="s">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="25" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1402,172 +1408,172 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="39" t="s">
+      <c r="E20" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="35"/>
+      <c r="F20" s="26"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="12" t="s">
+      <c r="C21" s="35"/>
+      <c r="D21" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="46" t="s">
+      <c r="E21" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="37"/>
+      <c r="F21" s="28"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="40" t="s">
+      <c r="A22" s="41"/>
+      <c r="B22" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="9" t="s">
+      <c r="C22" s="32"/>
+      <c r="D22" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="48" t="s">
+      <c r="E22" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="37"/>
+      <c r="F22" s="28"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="40" t="s">
+      <c r="A23" s="41"/>
+      <c r="B23" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11" t="s">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="48" t="s">
+      <c r="E23" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F23" s="37"/>
+      <c r="F23" s="28"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="8" t="s">
+      <c r="A24" s="41"/>
+      <c r="B24" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="48"/>
-      <c r="F24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="28"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="8" t="s">
+      <c r="A25" s="41"/>
+      <c r="B25" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="48"/>
-      <c r="F25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="28"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="49"/>
-      <c r="B26" s="14" t="s">
+      <c r="A26" s="42"/>
+      <c r="B26" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="50" t="s">
+      <c r="C26" s="13"/>
+      <c r="D26" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="51"/>
-      <c r="F26" s="37"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="28"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="36"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="37"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="28"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="37"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="28"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="37"/>
+      <c r="A29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="28"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="36"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="37"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="28"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="37"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="28"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="37"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="28"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="F33" s="4"/>
+      <c r="A33" s="27"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="36"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="F34" s="4"/>
+      <c r="A34" s="27"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="36"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
+      <c r="A35" s="27"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1582,7 +1588,7 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="F11:F14"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>